<commit_message>
fixed some problems pws
</commit_message>
<xml_diff>
--- a/performance_test/LEVIATHAN.xlsx
+++ b/performance_test/LEVIATHAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\Thesis\DBV-ISP\DBV-ISP-Miner\performance_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70999864-FD1B-4A46-8BD2-D8D659B20166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066899ED-C013-4AC6-912B-FA70E54DA198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +518,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="2">
-        <v>441</v>
+        <v>21</v>
       </c>
       <c r="K5" s="3"/>
     </row>
@@ -825,11 +825,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="A11:C11"/>
@@ -840,6 +835,11 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>